<commit_message>
conteo de participantes con correos enviados
</commit_message>
<xml_diff>
--- a/docs/formatos/CorreosParticipantes.xlsx
+++ b/docs/formatos/CorreosParticipantes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -35,15 +35,19 @@
   </si>
   <si>
     <t xml:space="preserve">Correo corporativo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total enviados</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="h:mm"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -156,7 +160,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -182,6 +186,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -209,10 +217,10 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.42"/>
@@ -282,14 +290,17 @@
       <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="F5" s="7"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -298,7 +309,7 @@
       <c r="L5" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F24" s="7"/>
+      <c r="F24" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>